<commit_message>
added new regression example
</commit_message>
<xml_diff>
--- a/assets/slides/acct3210/S3/Problem2and3.xlsx
+++ b/assets/slides/acct3210/S3/Problem2and3.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1970BF5-6E42-480F-B6AC-401003465ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shamussiothrun/ArthurHowardMorris.github.io/assets/slides/acct3210/S3/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6494A22-15CC-664A-A4EC-CA66B59BE7A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="76800" windowHeight="43200" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blank" sheetId="1" r:id="rId1"/>
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="56">
   <si>
     <t>Month</t>
   </si>
@@ -121,6 +126,90 @@
   <si>
     <t>December</t>
   </si>
+  <si>
+    <t>SUMMARY OUTPUT</t>
+  </si>
+  <si>
+    <t>Regression Statistics</t>
+  </si>
+  <si>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>Lower 95.0%</t>
+  </si>
+  <si>
+    <t>Upper 95.0%</t>
+  </si>
+  <si>
+    <t>RESIDUAL OUTPUT</t>
+  </si>
+  <si>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t>Predicted Operating Costs</t>
+  </si>
+  <si>
+    <t>Residuals</t>
+  </si>
 </sst>
 </file>
 
@@ -129,7 +218,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +239,14 @@
       <name val="Helvetica Neue"/>
       <charset val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -165,7 +262,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -173,29 +270,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -690,6 +815,12 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.4612700770500217E-2"/>
+                  <c:y val="-6.9363020196851144E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1896,6 +2027,601 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Miles  Residual Plot</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'p3 plot'!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>3420</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5310</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5410</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8440</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9320</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8910</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8870</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10980</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4980</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4480</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2980</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'p3 plot'!$K$25:$K$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>-24.329234231695807</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-94.196803105760637</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.360468382384056</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-78.554205526831083</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-74.450216431157514</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-20.135029532550789</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-7.9579381278088022</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>79.200490272044817</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>314.76420098336177</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>57.70165255490906</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-72.022156457361802</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-85.381228779532535</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8AB7-4341-B694-E31C1B2D78B9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="295309823"/>
+        <c:axId val="295273471"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="295309823"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Miles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="295273471"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="295273471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Residuals</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="295309823"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Miles Line Fit  Plot</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Operating Costs</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'p3 plot'!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>3420</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5310</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5410</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8440</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9320</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8910</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8870</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10980</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4980</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4480</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2980</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'p3 plot'!$C$2:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)">
+                  <c:v>471</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>609</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>742</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>774</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>784</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>986</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>895</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>651</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>481</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>386</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-24B7-464C-A167-24A2B992C8E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Predicted Operating Costs</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'p3 plot'!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>3420</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5310</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5410</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8440</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9320</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8910</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8870</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10980</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4980</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5220</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4480</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2980</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'p3 plot'!$J$25:$J$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>495.32923423169581</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>598.19680310576064</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>603.63953161761594</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>768.55420552683108</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>816.45021643115751</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>794.13502953255079</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>791.9579381278088</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>906.79950972795518</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>580.23579901663823</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>593.29834744509094</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>553.0221564573618</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>471.38122877953253</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-24B7-464C-A167-24A2B992C8E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="557797136"/>
+        <c:axId val="557799136"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="557797136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Miles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="557799136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="557799136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Operating Costs</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="557797136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -12063,6 +12789,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>177799</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>407737</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>93578</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{847EC493-66DF-5FE2-F8F9-C324D21678AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>607596</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>193173</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>120316</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>40104</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{791EB49C-DF76-542A-455D-B8E9B486011F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -12367,7 +13165,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12381,12 +13179,12 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.5">
+    <row r="1" spans="1:4" ht="27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12400,7 +13198,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -12414,7 +13212,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -12428,7 +13226,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -12442,7 +13240,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -12456,7 +13254,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -12470,7 +13268,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -12484,7 +13282,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -12498,7 +13296,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -12512,7 +13310,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -12539,12 +13337,12 @@
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5">
+    <row r="1" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12561,7 +13359,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -12579,7 +13377,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -12597,7 +13395,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -12615,7 +13413,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -12633,7 +13431,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -12651,7 +13449,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -12669,7 +13467,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -12687,7 +13485,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -12705,7 +13503,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -12736,13 +13534,13 @@
       <selection activeCell="B1" sqref="B1:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.5">
+    <row r="1" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12759,7 +13557,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -12780,7 +13578,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -12801,7 +13599,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -12822,7 +13620,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -12843,7 +13641,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -12861,7 +13659,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -12879,7 +13677,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -12897,7 +13695,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -12915,7 +13713,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -12947,13 +13745,13 @@
       <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.5">
+    <row r="1" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12970,7 +13768,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -12991,7 +13789,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -13012,7 +13810,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -13033,7 +13831,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -13054,7 +13852,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -13075,7 +13873,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -13093,7 +13891,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -13111,7 +13909,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -13129,7 +13927,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -13147,7 +13945,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="25.5">
+    <row r="59" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
@@ -13164,7 +13962,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -13185,7 +13983,7 @@
         <v>2113</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>20</v>
       </c>
@@ -13206,7 +14004,7 @@
         <v>2406</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>21</v>
       </c>
@@ -13239,7 +14037,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13253,13 +14051,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.5">
+    <row r="1" spans="1:4" ht="27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13273,7 +14071,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -13287,7 +14085,7 @@
         <v>3420</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -13301,7 +14099,7 @@
         <v>5310</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -13315,7 +14113,7 @@
         <v>5410</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -13329,7 +14127,7 @@
         <v>8440</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -13343,7 +14141,7 @@
         <v>9320</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -13357,7 +14155,7 @@
         <v>8910</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -13371,7 +14169,7 @@
         <v>8870</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -13385,7 +14183,7 @@
         <v>10980</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -13399,7 +14197,7 @@
         <v>4980</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
@@ -13413,7 +14211,7 @@
         <v>5220</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -13427,7 +14225,7 @@
         <v>4480</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
@@ -13454,13 +14252,13 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" customWidth="1"/>
+    <col min="3" max="4" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5">
+    <row r="1" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13477,7 +14275,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -13495,7 +14293,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -13513,7 +14311,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -13531,7 +14329,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -13549,7 +14347,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -13567,7 +14365,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -13585,7 +14383,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -13603,7 +14401,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -13621,7 +14419,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -13639,7 +14437,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
@@ -13657,7 +14455,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -13675,7 +14473,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
@@ -13700,19 +14498,21 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2CBA3B0-196D-4B0D-869B-8C9F0343F141}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="Q34" sqref="Q34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" customWidth="1"/>
+    <col min="3" max="4" width="11.5" customWidth="1"/>
+    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5">
+    <row r="1" spans="1:17" ht="27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13728,8 +14528,11 @@
       <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -13747,7 +14550,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -13764,8 +14567,12 @@
         <f t="shared" ref="E3:E13" si="0">C3+D3</f>
         <v>842</v>
       </c>
+      <c r="I3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="10"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -13782,8 +14589,14 @@
         <f t="shared" si="0"/>
         <v>952</v>
       </c>
+      <c r="I4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0.7816254808377463</v>
+      </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -13800,8 +14613,14 @@
         <f t="shared" si="0"/>
         <v>1037</v>
       </c>
+      <c r="I5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.61093839229483815</v>
+      </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -13818,8 +14637,14 @@
         <f t="shared" si="0"/>
         <v>1036</v>
       </c>
+      <c r="I6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0.57203223152432192</v>
+      </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -13836,8 +14661,14 @@
         <f t="shared" si="0"/>
         <v>985</v>
       </c>
+      <c r="I7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="7">
+        <v>119.5122905551185</v>
+      </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -13854,8 +14685,14 @@
         <f t="shared" si="0"/>
         <v>960</v>
       </c>
+      <c r="I8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="8">
+        <v>12</v>
+      </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -13873,7 +14710,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -13890,8 +14727,11 @@
         <f t="shared" si="0"/>
         <v>1177</v>
       </c>
+      <c r="I10" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
@@ -13908,8 +14748,24 @@
         <f t="shared" si="0"/>
         <v>1045</v>
       </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="N11" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -13926,8 +14782,26 @@
         <f t="shared" si="0"/>
         <v>862</v>
       </c>
+      <c r="I12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="7">
+        <v>1</v>
+      </c>
+      <c r="K12" s="7">
+        <v>224287.04072935597</v>
+      </c>
+      <c r="L12" s="7">
+        <v>224287.04072935597</v>
+      </c>
+      <c r="M12" s="7">
+        <v>15.702870193191066</v>
+      </c>
+      <c r="N12" s="7">
+        <v>2.6748017211876527E-3</v>
+      </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
@@ -13943,6 +14817,269 @@
       <c r="E13" s="3">
         <f t="shared" si="0"/>
         <v>900</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="7">
+        <v>10</v>
+      </c>
+      <c r="K13" s="7">
+        <v>142831.87593731066</v>
+      </c>
+      <c r="L13" s="7">
+        <v>14283.187593731065</v>
+      </c>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+    </row>
+    <row r="14" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="8">
+        <v>11</v>
+      </c>
+      <c r="K14" s="8">
+        <v>367118.91666666663</v>
+      </c>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+    </row>
+    <row r="15" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I16" s="9"/>
+      <c r="J16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="P16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q16" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="9:17" x14ac:dyDescent="0.2">
+      <c r="I17" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J17" s="7">
+        <v>309.18791912624511</v>
+      </c>
+      <c r="K17" s="7">
+        <v>96.053186165298968</v>
+      </c>
+      <c r="L17" s="7">
+        <v>3.2189241343245008</v>
+      </c>
+      <c r="M17" s="7">
+        <v>9.1918955747625833E-3</v>
+      </c>
+      <c r="N17" s="7">
+        <v>95.16808317427197</v>
+      </c>
+      <c r="O17" s="7">
+        <v>523.20775507821827</v>
+      </c>
+      <c r="P17" s="7">
+        <v>95.16808317427197</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>523.20775507821827</v>
+      </c>
+    </row>
+    <row r="18" spans="9:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="8">
+        <v>5.4427285118552833E-2</v>
+      </c>
+      <c r="K18" s="8">
+        <v>1.3734952174856128E-2</v>
+      </c>
+      <c r="L18" s="8">
+        <v>3.9626847203873101</v>
+      </c>
+      <c r="M18" s="8">
+        <v>2.67480172118766E-3</v>
+      </c>
+      <c r="N18" s="8">
+        <v>2.3823904547582517E-2</v>
+      </c>
+      <c r="O18" s="8">
+        <v>8.5030665689523152E-2</v>
+      </c>
+      <c r="P18" s="8">
+        <v>2.3823904547582517E-2</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>8.5030665689523152E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="9:17" x14ac:dyDescent="0.2">
+      <c r="I22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="9:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="9:17" x14ac:dyDescent="0.2">
+      <c r="I24" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="9:17" x14ac:dyDescent="0.2">
+      <c r="I25" s="7">
+        <v>1</v>
+      </c>
+      <c r="J25" s="7">
+        <v>495.32923423169581</v>
+      </c>
+      <c r="K25" s="7">
+        <v>-24.329234231695807</v>
+      </c>
+    </row>
+    <row r="26" spans="9:17" x14ac:dyDescent="0.2">
+      <c r="I26" s="7">
+        <v>2</v>
+      </c>
+      <c r="J26" s="7">
+        <v>598.19680310576064</v>
+      </c>
+      <c r="K26" s="7">
+        <v>-94.196803105760637</v>
+      </c>
+    </row>
+    <row r="27" spans="9:17" x14ac:dyDescent="0.2">
+      <c r="I27" s="7">
+        <v>3</v>
+      </c>
+      <c r="J27" s="7">
+        <v>603.63953161761594</v>
+      </c>
+      <c r="K27" s="7">
+        <v>5.360468382384056</v>
+      </c>
+    </row>
+    <row r="28" spans="9:17" x14ac:dyDescent="0.2">
+      <c r="I28" s="7">
+        <v>4</v>
+      </c>
+      <c r="J28" s="7">
+        <v>768.55420552683108</v>
+      </c>
+      <c r="K28" s="7">
+        <v>-78.554205526831083</v>
+      </c>
+    </row>
+    <row r="29" spans="9:17" x14ac:dyDescent="0.2">
+      <c r="I29" s="7">
+        <v>5</v>
+      </c>
+      <c r="J29" s="7">
+        <v>816.45021643115751</v>
+      </c>
+      <c r="K29" s="7">
+        <v>-74.450216431157514</v>
+      </c>
+    </row>
+    <row r="30" spans="9:17" x14ac:dyDescent="0.2">
+      <c r="I30" s="7">
+        <v>6</v>
+      </c>
+      <c r="J30" s="7">
+        <v>794.13502953255079</v>
+      </c>
+      <c r="K30" s="7">
+        <v>-20.135029532550789</v>
+      </c>
+    </row>
+    <row r="31" spans="9:17" x14ac:dyDescent="0.2">
+      <c r="I31" s="7">
+        <v>7</v>
+      </c>
+      <c r="J31" s="7">
+        <v>791.9579381278088</v>
+      </c>
+      <c r="K31" s="7">
+        <v>-7.9579381278088022</v>
+      </c>
+    </row>
+    <row r="32" spans="9:17" x14ac:dyDescent="0.2">
+      <c r="I32" s="7">
+        <v>8</v>
+      </c>
+      <c r="J32" s="7">
+        <v>906.79950972795518</v>
+      </c>
+      <c r="K32" s="7">
+        <v>79.200490272044817</v>
+      </c>
+    </row>
+    <row r="33" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I33" s="7">
+        <v>9</v>
+      </c>
+      <c r="J33" s="7">
+        <v>580.23579901663823</v>
+      </c>
+      <c r="K33" s="7">
+        <v>314.76420098336177</v>
+      </c>
+    </row>
+    <row r="34" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I34" s="7">
+        <v>10</v>
+      </c>
+      <c r="J34" s="7">
+        <v>593.29834744509094</v>
+      </c>
+      <c r="K34" s="7">
+        <v>57.70165255490906</v>
+      </c>
+    </row>
+    <row r="35" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I35" s="7">
+        <v>11</v>
+      </c>
+      <c r="J35" s="7">
+        <v>553.0221564573618</v>
+      </c>
+      <c r="K35" s="7">
+        <v>-72.022156457361802</v>
+      </c>
+    </row>
+    <row r="36" spans="9:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I36" s="8">
+        <v>12</v>
+      </c>
+      <c r="J36" s="8">
+        <v>471.38122877953253</v>
+      </c>
+      <c r="K36" s="8">
+        <v>-85.381228779532535</v>
       </c>
     </row>
   </sheetData>

</xml_diff>